<commit_message>
Projet de visualition de donnée One Piece Explorer
</commit_message>
<xml_diff>
--- a/Donnee/SortieMangaAnime/SortieMangaAnime.xlsx
+++ b/Donnee/SortieMangaAnime/SortieMangaAnime.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\assef\OneDrive\Bureau\1HEIG\semetre 2\VisualDonne\Projet\Site\Donnee\SortieMangaAnime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F31170B-0483-4041-A894-5C2AE442295D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8857B3-5100-41F8-AB85-6458C653EFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A46143C2-9548-4B63-B1E3-897DF93E5C8D}"/>
   </bookViews>
@@ -36,90 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Année</t>
   </si>
   <si>
     <t>Chapitres</t>
-  </si>
-  <si>
-    <t>22 - 44</t>
-  </si>
-  <si>
-    <t>45 - 69</t>
-  </si>
-  <si>
-    <t>70 - 95</t>
-  </si>
-  <si>
-    <t>96 - 122</t>
-  </si>
-  <si>
-    <t>123 - 154</t>
-  </si>
-  <si>
-    <t>155 - 186</t>
-  </si>
-  <si>
-    <t>187 - 218</t>
-  </si>
-  <si>
-    <t>219 - 254</t>
-  </si>
-  <si>
-    <t>255 - 290</t>
-  </si>
-  <si>
-    <t>291 - 325</t>
-  </si>
-  <si>
-    <t>326 - 357</t>
-  </si>
-  <si>
-    <t>358 - 391</t>
-  </si>
-  <si>
-    <t>392 - 441</t>
-  </si>
-  <si>
-    <t>442 - 490</t>
-  </si>
-  <si>
-    <t>491 - 541</t>
-  </si>
-  <si>
-    <t>542 - 597</t>
-  </si>
-  <si>
-    <t>598 - 651</t>
-  </si>
-  <si>
-    <t>652 - 704</t>
-  </si>
-  <si>
-    <t>705 - 757</t>
-  </si>
-  <si>
-    <t>758 - 907</t>
-  </si>
-  <si>
-    <t>908 - 959</t>
-  </si>
-  <si>
-    <t>960 - 1008</t>
-  </si>
-  <si>
-    <t>1009 - 1068</t>
-  </si>
-  <si>
-    <t>1069 - aujourd'hui</t>
-  </si>
-  <si>
-    <t>1 :,8</t>
-  </si>
-  <si>
-    <t>9 :,21</t>
   </si>
 </sst>
 </file>
@@ -225,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -238,9 +160,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCCEE27-0972-4969-A058-9ECC4C67A265}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,208 +503,208 @@
       <c r="A2" s="1">
         <v>1997</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
+      <c r="B2" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1998</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
+      <c r="B3" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1999</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
+      <c r="B4" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2000</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
+      <c r="B5" s="2">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2001</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
+      <c r="B6" s="2">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2002</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
+      <c r="B7" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2003</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
+      <c r="B8" s="2">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2004</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
+      <c r="B9" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2005</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
+      <c r="B10" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2006</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
+      <c r="B11" s="2">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2007</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
+      <c r="B12" s="2">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2008</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
+      <c r="B13" s="2">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2009</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
+      <c r="B14" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2010</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
+      <c r="B15" s="2">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2011</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
+      <c r="B16" s="2">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2012</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
+      <c r="B17" s="2">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2013</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>16</v>
+      <c r="B18" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2014</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>17</v>
+      <c r="B19" s="2">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2015</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>18</v>
+      <c r="B20" s="2">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2016</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>19</v>
+      <c r="B21" s="2">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2017</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
+      <c r="B22" s="2">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2018</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>21</v>
+      <c r="B23" s="2">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2019</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>22</v>
+      <c r="B24" s="2">
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2020</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>23</v>
+      <c r="B25" s="2">
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2021</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>24</v>
+      <c r="B26" s="2">
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2022</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>25</v>
+      <c r="B27" s="2">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>